<commit_message>
CP-002 - Crear turno valido
</commit_message>
<xml_diff>
--- a/Log Pruebas.xlsx
+++ b/Log Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TIO\TPE-TIO-2024\proyecto-tio-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80806A66-1CFA-4E5E-A7C2-DD3B0C69834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D763474-CD9E-43D5-B163-647B7312856F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA0D0AD8-70AC-4ECB-9E10-FFED996A0ED6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>Proyecto Sitio Veterinaria</t>
+  </si>
+  <si>
+    <t>CP-002</t>
+  </si>
+  <si>
+    <t>Crear un turno valido</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>Funciono Correctamente</t>
   </si>
 </sst>
 </file>
@@ -348,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,9 +378,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -380,6 +390,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,7 +731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE2AA61-40D2-413D-BEAC-51C04D6FE6D3}">
-  <dimension ref="B1:F39"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -725,22 +742,22 @@
     <col min="1" max="1" width="3.21875" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.21875" customWidth="1"/>
     <col min="8" max="16384" width="11.5546875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -777,67 +794,77 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="10"/>
+      <c r="B5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="17">
+        <v>45595</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="10"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="9"/>
     </row>
     <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3"/>
     <row r="17" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
se actualiza repo local
</commit_message>
<xml_diff>
--- a/Log Pruebas.xlsx
+++ b/Log Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TIO\TPE-TIO-2024\proyecto-tio-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80806A66-1CFA-4E5E-A7C2-DD3B0C69834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E375A7-4D77-4027-8FF6-7A967F3259A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA0D0AD8-70AC-4ECB-9E10-FFED996A0ED6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -66,13 +66,40 @@
   </si>
   <si>
     <t>Proyecto Sitio Veterinaria</t>
+  </si>
+  <si>
+    <t>CP-002</t>
+  </si>
+  <si>
+    <t>Crear un turno valido</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>Funciono Correctamente</t>
+  </si>
+  <si>
+    <t>CP-003</t>
+  </si>
+  <si>
+    <t>CP-004</t>
+  </si>
+  <si>
+    <t>Eliminar un cliente</t>
+  </si>
+  <si>
+    <t>Se creo turno</t>
+  </si>
+  <si>
+    <t>Crear un turno con fecha invalida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +123,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +149,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -348,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,11 +405,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -380,6 +424,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE2AA61-40D2-413D-BEAC-51C04D6FE6D3}">
-  <dimension ref="B1:F39"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -725,24 +770,35 @@
     <col min="1" max="1" width="3.21875" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.21875" customWidth="1"/>
     <col min="8" max="16384" width="11.5546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="18"/>
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,8 +814,10 @@
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -775,71 +833,128 @@
       <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="9"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="18"/>
+      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="14">
+        <v>45595</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="18"/>
+      <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="14">
+        <v>45596</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="14">
+        <v>45596</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
     <row r="17" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="19" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
@@ -863,10 +978,17 @@
     <row r="37" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="38" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="39" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="41" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="42" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="43" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="44" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="45" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
se cambio estado en la CP-003
</commit_message>
<xml_diff>
--- a/Log Pruebas.xlsx
+++ b/Log Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TIO\TPE-TIO-2024\proyecto-tio-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E375A7-4D77-4027-8FF6-7A967F3259A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B45392-3A3E-413D-BB86-026112913AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA0D0AD8-70AC-4ECB-9E10-FFED996A0ED6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Caso de Prueba</t>
   </si>
@@ -89,10 +89,13 @@
     <t>Eliminar un cliente</t>
   </si>
   <si>
-    <t>Se creo turno</t>
-  </si>
-  <si>
     <t>Crear un turno con fecha invalida</t>
+  </si>
+  <si>
+    <t>Resuelto</t>
+  </si>
+  <si>
+    <t>Se mostro error turno invalido</t>
   </si>
 </sst>
 </file>
@@ -415,6 +418,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,7 +428,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,7 +765,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -772,33 +775,33 @@
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.21875" customWidth="1"/>
     <col min="8" max="16384" width="11.5546875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="18"/>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="18"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,10 +817,10 @@
       <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
@@ -833,10 +836,10 @@
       <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="12" t="s">
         <v>10</v>
       </c>
@@ -852,29 +855,29 @@
       <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="14">
-        <v>45596</v>
+        <v>45597</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="18"/>
+        <v>19</v>
+      </c>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
@@ -890,70 +893,70 @@
       <c r="F7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="12"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="12"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="12"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="12"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="12"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="18"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="13"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="18"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="17" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="18" customFormat="1" hidden="1" x14ac:dyDescent="0.3"/>

</xml_diff>